<commit_message>
split up row_as_str column
</commit_message>
<xml_diff>
--- a/Scripts/copy_counts.xlsx
+++ b/Scripts/copy_counts.xlsx
@@ -14,39 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
-  <si>
-    <t>row_as_str</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+  <si>
+    <t>../Data/Data_0_Synergy.csv</t>
+  </si>
+  <si>
+    <t>../Data/Data_1_old_replication.csv</t>
+  </si>
+  <si>
+    <t>../Data/Data_2_old_comprehensive.csv</t>
+  </si>
+  <si>
+    <t>Data_4a_snowballing.csv</t>
+  </si>
+  <si>
+    <t>Data_3a_inlusion_criteria.csv</t>
+  </si>
+  <si>
+    <t>Data_3b_includedrecords_top88.csv</t>
+  </si>
+  <si>
+    <t>Data_3c_active_learning_total1000.csv</t>
   </si>
   <si>
     <t>frequency</t>
-  </si>
-  <si>
-    <t>../Data/Data_0_Synergy.csv</t>
-  </si>
-  <si>
-    <t>../Data/Data_1_old_replication.csv</t>
-  </si>
-  <si>
-    <t>../Data/Data_2_old_comprehensive.csv</t>
-  </si>
-  <si>
-    <t>Data_4a_snowballing.csv</t>
-  </si>
-  <si>
-    <t>Data_3a_inlusion_criteria.csv</t>
-  </si>
-  <si>
-    <t>Data_3b_includedrecords_top88.csv</t>
-  </si>
-  <si>
-    <t>Data_3c_active_learning_total1000.csv</t>
-  </si>
-  <si>
-    <t>1000000</t>
-  </si>
-  <si>
-    <t>1110000</t>
   </si>
   <si>
     <t>1</t>
@@ -410,13 +401,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,66 +432,57 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>